<commit_message>
Bảng phân công công việc
có chỉnh sửa
</commit_message>
<xml_diff>
--- a/Phancong.xlsx
+++ b/Phancong.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10170" windowHeight="4485"/>
   </bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>STT</t>
   </si>
@@ -109,13 +109,19 @@
   </si>
   <si>
     <t>Xây dựng phần mềm quản lý kho</t>
+  </si>
+  <si>
+    <t>Leader : LanNguyen28</t>
+  </si>
+  <si>
+    <t>PHẦN MỀM QUẢN LÝ KHO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +153,20 @@
       <b/>
       <sz val="14"/>
       <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -199,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -225,12 +245,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,20 +549,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="A1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">

</xml_diff>